<commit_message>
[Members] Display more info about members
Co-Authored-By: Ven <vendicated@riseup.net>
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,19 +28,46 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keanu Timmermans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web/App dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Developer</t>
   </si>
   <si>
     <t xml:space="preserve">Njord-Romijn Witsiers</t>
   </si>
   <si>
+    <t xml:space="preserve">Arduino dev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lars Leijssen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[TBD]</t>
   </si>
   <si>
     <t xml:space="preserve">Dion Welles</t>
   </si>
   <si>
+    <t xml:space="preserve">Device manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systems and Devices</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tom Vergeldt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network manager</t>
   </si>
 </sst>
 </file>
@@ -150,13 +177,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1006"/>
+  <dimension ref="A1:D1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
   </cols>
@@ -168,45 +195,81 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>15</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>17</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>18</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[Members] Calculate member age from birth date
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Keanu Timmermans</t>
   </si>
   <si>
+    <t xml:space="preserve">28/Nov/05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Web/App dev</t>
   </si>
   <si>
@@ -46,16 +49,25 @@
     <t xml:space="preserve">Njord-Romijn Witsiers</t>
   </si>
   <si>
+    <t xml:space="preserve">08/Mar/04</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arduino dev</t>
   </si>
   <si>
     <t xml:space="preserve">Lars Leijssen</t>
   </si>
   <si>
+    <t xml:space="preserve">13/May/05</t>
+  </si>
+  <si>
     <t xml:space="preserve">[TBD]</t>
   </si>
   <si>
     <t xml:space="preserve">Dion Welles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/Jan/03</t>
   </si>
   <si>
     <t xml:space="preserve">Device manager</t>
@@ -65,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tom Vergeldt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/Aug/02</t>
   </si>
   <si>
     <t xml:space="preserve">Network manager</t>
@@ -180,12 +195,12 @@
   <dimension ref="A1:D1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -195,10 +210,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -206,70 +221,70 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="n">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="n">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>13</v>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,13 +3289,13 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B1006" type="whole">
-      <formula1>10</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:A1006" type="none">
       <formula1>ISTEXT(A2:A6)</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B1:B1006" type="none">
+      <formula1>10</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[Member] WIP: Display all member info on page
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
+    <t xml:space="preserve">DoB</t>
   </si>
   <si>
     <t xml:space="preserve">Role</t>
@@ -34,6 +34,24 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
+    <t xml:space="preserve">OfficeNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FavColour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keanu Timmermans</t>
   </si>
   <si>
@@ -46,6 +64,21 @@
     <t xml:space="preserve">Software Developer</t>
   </si>
   <si>
+    <t xml:space="preserve">112-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keanucode@c2dl.info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmeren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blauw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 honden</t>
+  </si>
+  <si>
     <t xml:space="preserve">Njord-Romijn Witsiers</t>
   </si>
   <si>
@@ -55,12 +88,30 @@
     <t xml:space="preserve">Arduino dev</t>
   </si>
   <si>
+    <t xml:space="preserve">Njord-Romijn.Witsiers@Student.GildeOpleidingen.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slapen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hond</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lars Leijssen</t>
   </si>
   <si>
     <t xml:space="preserve">13/May/05</t>
   </si>
   <si>
+    <t xml:space="preserve">Lars.Leijssen@Student.GildeOpleidingen.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atletiek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donkergroen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dion Welles</t>
   </si>
   <si>
@@ -73,6 +124,15 @@
     <t xml:space="preserve">Systems and Devices</t>
   </si>
   <si>
+    <t xml:space="preserve">Dion.Welles@Student.GildeOpleidingen.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kat</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tom Vergeldt</t>
   </si>
   <si>
@@ -80,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Network manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom.Vergeldt@Student.GildeOpleidingen.nl</t>
   </si>
 </sst>
 </file>
@@ -90,7 +153,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -111,6 +174,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,6 +239,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,13 +263,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1006"/>
+  <dimension ref="A1:J1006"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
   </cols>
@@ -213,75 +287,171 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>621654958</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>630743511</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>683561065</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>681814608</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,6 +3465,13 @@
       <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="keanucode@c2dl.info"/>
+    <hyperlink ref="F3" r:id="rId2" display="Njord-Romijn.Witsiers@Student.GildeOpleidingen.nl"/>
+    <hyperlink ref="F4" r:id="rId3" display="Lars.Leijssen@Student.GildeOpleidingen.nl"/>
+    <hyperlink ref="F5" r:id="rId4" display="Dion.Welles@Student.GildeOpleidingen.nl"/>
+    <hyperlink ref="F6" r:id="rId5" display="Tom.Vergeldt@Student.GildeOpleidingen.nl"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
[Member] Display email as URL
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tom.Vergeldt@Student.GildeOpleidingen.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness, YuGiOh, Pokemon, karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donkerblauw</t>
   </si>
 </sst>
 </file>
@@ -266,10 +272,10 @@
   <dimension ref="A1:J1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
   </cols>
@@ -287,22 +293,22 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -319,22 +325,22 @@
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="3" t="n">
         <v>621654958</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -351,22 +357,22 @@
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="3" t="n">
         <v>630743511</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -383,22 +389,22 @@
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="3" t="n">
         <v>683561065</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -415,22 +421,22 @@
       <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="3" t="n">
         <v>681814608</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -447,11 +453,23 @@
       <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>638478508</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>